<commit_message>
cambio logica de asignacion PREPAID (60) y mas de 1 cuota CREDIT (10). Genero DEVBOTON vacio
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1818072874.0</v>
+        <v>1638041672.0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -386,7 +386,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>1822225502.0</v>
+        <v>1611264484.0</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -394,7 +394,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>1195849953.0</v>
+        <v>1650221344.0</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -402,7 +402,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>1206482622.0</v>
+        <v>1908704539.0</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>1155066173.0</v>
+        <v>1611905756.0</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1547902419.0</v>
+        <v>1772895896.0</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -428,5 +428,14 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update de procesador_API_Menta para luego de conectarme a la API, generar el archivo del BIND, tanto BOTON como DEVBOTON (vacio) y el archivo excel de cuotas
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1638041672.0</v>
+        <v>151979169</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -386,15 +386,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>1611264484.0</v>
+        <v>726896511</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>1650221344.0</v>
+        <v>550338825</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -402,7 +402,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>1908704539.0</v>
+        <v>764228034</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>1611905756.0</v>
+        <v>758146980</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -418,10 +418,66 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1772895896.0</v>
+        <v>171935222</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>20645182</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>79418400</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>641239853</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>110151679</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>749067789</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>189153073</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>254395074</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readme file con requisitos de instalacion y ejecucion
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>151979169</v>
+        <v>828271183</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -386,7 +386,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>726896511</v>
+        <v>668066389</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -394,7 +394,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>550338825</v>
+        <v>669436101</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -402,7 +402,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>764228034</v>
+        <v>550712337</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>758146980</v>
+        <v>439469821</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -418,23 +418,23 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>171935222</v>
+        <v>488102342</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>20645182</v>
+        <v>985252614</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>79418400</v>
+        <v>332987301</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>641239853</v>
+        <v>638201176</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>110151679</v>
+        <v>592586767</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -458,26 +458,10 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>749067789</v>
+        <v>961249559</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>189153073</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>254395074</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correccion de bug al armar la hora de la fechastart. Captura de fechas de inicio y fin y duracion de proceso
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,90 +378,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>828271183</v>
+        <v>1872782709</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>668066389</v>
+        <v>302618540</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>669436101</v>
+        <v>1002639483</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>550712337</v>
+        <v>816818518</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>439469821</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>488102342</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>985252614</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>332987301</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>638201176</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>592586767</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>961249559</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega al log la cantidad de trx descartartadas por estado FAILED, REVERSED o REJECTE
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,34 +378,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1872782709</v>
+        <v>151979169</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>302618540</v>
+        <v>726896511</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>1002639483</v>
+        <v>550338825</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>816818518</v>
+        <v>764228034</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>758146980</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>171935222</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>20645182</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>79418400</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>641239853</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>110151679</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>749067789</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>189153073</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>254395074</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inclusion de 2 campos nuevos en liquidaciondetalle 'costomipyme e IVAcostomipyme' para reflejar el FINANCIAL_COST que baja de Menta. Se fuerza el calculo de % de mipyme y se fuerza el % del 10.5 para el IVA del costo mipyme. Corrección de defectos tras las pruebas.
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>151979169</v>
+        <v>63582208</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -386,7 +386,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>726896511</v>
+        <v>948403273</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -394,23 +394,23 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>550338825</v>
+        <v>530936366</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>764228034</v>
+        <v>852350050</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>758146980</v>
+        <v>690758213</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -418,66 +418,18 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>171935222</v>
+        <v>517999539</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>20645182</v>
+        <v>504974250</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>79418400</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>641239853</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>110151679</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>749067789</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>189153073</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>254395074</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizo con version productiva
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,58 +378,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>63582208</v>
+        <v>580644304</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>948403273</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>530936366</v>
-      </c>
-      <c r="B4">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>852350050</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>690758213</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>517999539</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>504974250</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en procesador_API_Menta, archivosdiarios.php y liquidaciondiaria.php para interactuar con el proyecto Orquestador desarrollado bajo Symfony
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -360,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,10 +378,90 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>580644304</v>
+        <v>48719471</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>407850697</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>610342243</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>77835143</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>416623687</v>
+      </c>
+      <c r="B6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>178820206</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>536241934</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>628217301</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>29435298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>262751091</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>363942941</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
procesador_API_Menta genera archivos vacios si no encuentra ventas para que no falle archivosdiarios.php
</commit_message>
<xml_diff>
--- a/api/archivocuotas.xlsx
+++ b/api/archivocuotas.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Cuotas" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,14 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>Transaccion</t>
-  </si>
-  <si>
-    <t>Cuotas</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,111 +353,14 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>48719471</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>407850697</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>610342243</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>77835143</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>416623687</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>178820206</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>536241934</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>628217301</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>29435298</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>262751091</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>363942941</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>